<commit_message>
iCommit de Abril 2022. Ya no se mira a Rot90
</commit_message>
<xml_diff>
--- a/WMM_All_configurations/MCBXFA_02_Inner_Iron_600_20220510-2/Roxie_vs_MM_NormalMCBXFA_02_Inner_Iron_600_20220510-2.xlsx
+++ b/WMM_All_configurations/MCBXFA_02_Inner_Iron_600_20220510-2/Roxie_vs_MM_NormalMCBXFA_02_Inner_Iron_600_20220510-2.xlsx
@@ -576,46 +576,46 @@
         <v>421.7675412068219</v>
       </c>
       <c r="D2">
-        <v>3.933099578022457</v>
+        <v>3.933099578022456</v>
       </c>
       <c r="E2">
         <v>-98.22389278735834</v>
       </c>
       <c r="F2">
-        <v>-0.4499586647880943</v>
+        <v>-0.4499586647880926</v>
       </c>
       <c r="G2">
-        <v>-8.964821934890297</v>
+        <v>-8.964821934890303</v>
       </c>
       <c r="H2">
-        <v>0.005872665162180496</v>
+        <v>0.005872665162181086</v>
       </c>
       <c r="I2">
-        <v>0.2780706887266789</v>
+        <v>0.2780706887266786</v>
       </c>
       <c r="J2">
-        <v>-0.108679837962031</v>
+        <v>-0.1086798379620302</v>
       </c>
       <c r="K2">
-        <v>0.359144459087455</v>
+        <v>0.3591444590874575</v>
       </c>
       <c r="L2">
-        <v>0.00744575824645229</v>
+        <v>0.007445758246456468</v>
       </c>
       <c r="M2">
-        <v>0.3494774226299343</v>
+        <v>0.3494774226299476</v>
       </c>
       <c r="N2">
-        <v>0.1645153716248129</v>
+        <v>0.1645153716247875</v>
       </c>
       <c r="O2">
-        <v>-0.3461642553629748</v>
+        <v>-0.3461642553630373</v>
       </c>
       <c r="P2">
-        <v>-0.0002162807604464084</v>
+        <v>-0.0002162807604438962</v>
       </c>
       <c r="Q2">
-        <v>-0.1234300518457799</v>
+        <v>-0.1234300518457798</v>
       </c>
       <c r="R2">
         <v>-0.2988425617549172</v>
@@ -674,46 +674,46 @@
         <v>2880.334169928937</v>
       </c>
       <c r="D3">
-        <v>8.030666472195492</v>
+        <v>8.030666472195493</v>
       </c>
       <c r="E3">
         <v>-102.9681621161403</v>
       </c>
       <c r="F3">
-        <v>-0.4769441691336769</v>
+        <v>-0.4769441691336742</v>
       </c>
       <c r="G3">
         <v>-40.71443721306763</v>
       </c>
       <c r="H3">
-        <v>0.3413972027342612</v>
+        <v>0.3413972027342639</v>
       </c>
       <c r="I3">
-        <v>-19.00848016858873</v>
+        <v>-19.00848016858874</v>
       </c>
       <c r="J3">
-        <v>0.04071829421918825</v>
+        <v>0.04071829421919065</v>
       </c>
       <c r="K3">
         <v>-6.083976774271058</v>
       </c>
       <c r="L3">
-        <v>-0.06643334236929041</v>
+        <v>-0.0664333423692916</v>
       </c>
       <c r="M3">
-        <v>-1.45411138237078</v>
+        <v>-1.454111382370782</v>
       </c>
       <c r="N3">
-        <v>-0.195431006606372</v>
+        <v>-0.1954310066064042</v>
       </c>
       <c r="O3">
-        <v>-0.3914503066764011</v>
+        <v>-0.3914503066763195</v>
       </c>
       <c r="P3">
-        <v>0.0007658153403677705</v>
+        <v>0.0007658153403914023</v>
       </c>
       <c r="Q3">
-        <v>-0.09094516599223262</v>
+        <v>-0.09094516599222514</v>
       </c>
       <c r="R3">
         <v>3883.249378802444</v>
@@ -772,46 +772,46 @@
         <v>10000</v>
       </c>
       <c r="D4">
-        <v>1.520601844193056</v>
+        <v>1.520601844193057</v>
       </c>
       <c r="E4">
         <v>-10.40025407585737</v>
       </c>
       <c r="F4">
-        <v>0.8312050572165446</v>
+        <v>0.8312050572165448</v>
       </c>
       <c r="G4">
-        <v>-8.380174487851768</v>
+        <v>-8.380174487851772</v>
       </c>
       <c r="H4">
-        <v>0.03729585551908479</v>
+        <v>0.03729585551908485</v>
       </c>
       <c r="I4">
-        <v>-0.7175660235358906</v>
+        <v>-0.7175660235358907</v>
       </c>
       <c r="J4">
-        <v>-0.06508710207152611</v>
+        <v>-0.06508710207152604</v>
       </c>
       <c r="K4">
         <v>0.8982796489936381</v>
       </c>
       <c r="L4">
-        <v>-0.3688488178457793</v>
+        <v>-0.3688488178457792</v>
       </c>
       <c r="M4">
-        <v>2.79181280931899</v>
+        <v>2.791812809318989</v>
       </c>
       <c r="N4">
-        <v>0.2857434155902019</v>
+        <v>0.2857434155902008</v>
       </c>
       <c r="O4">
-        <v>-1.556032338575846</v>
+        <v>-1.556032338575843</v>
       </c>
       <c r="P4">
-        <v>-0.07246337697313605</v>
+        <v>-0.07246337697313572</v>
       </c>
       <c r="Q4">
-        <v>0.2088441934989191</v>
+        <v>0.2088441934989194</v>
       </c>
       <c r="R4">
         <v>9999.846038205334</v>
@@ -870,46 +870,46 @@
         <v>10000</v>
       </c>
       <c r="D5">
-        <v>1.520601844193056</v>
+        <v>1.520601844193057</v>
       </c>
       <c r="E5">
         <v>-10.40025407585737</v>
       </c>
       <c r="F5">
-        <v>0.8312050572165446</v>
+        <v>0.8312050572165448</v>
       </c>
       <c r="G5">
-        <v>-8.380174487851768</v>
+        <v>-8.380174487851772</v>
       </c>
       <c r="H5">
-        <v>0.03729585551908479</v>
+        <v>0.03729585551908485</v>
       </c>
       <c r="I5">
-        <v>-0.7175660235358906</v>
+        <v>-0.7175660235358907</v>
       </c>
       <c r="J5">
-        <v>-0.06508710207152611</v>
+        <v>-0.06508710207152604</v>
       </c>
       <c r="K5">
         <v>0.8982796489936381</v>
       </c>
       <c r="L5">
-        <v>-0.3688488178457793</v>
+        <v>-0.3688488178457792</v>
       </c>
       <c r="M5">
-        <v>2.79181280931899</v>
+        <v>2.791812809318989</v>
       </c>
       <c r="N5">
-        <v>0.2857434155902019</v>
+        <v>0.2857434155902008</v>
       </c>
       <c r="O5">
-        <v>-1.556032338575846</v>
+        <v>-1.556032338575843</v>
       </c>
       <c r="P5">
-        <v>-0.07246337697313605</v>
+        <v>-0.07246337697313572</v>
       </c>
       <c r="Q5">
-        <v>0.2088441934989191</v>
+        <v>0.2088441934989194</v>
       </c>
       <c r="R5">
         <v>10000</v>
@@ -968,46 +968,46 @@
         <v>10000</v>
       </c>
       <c r="D6">
-        <v>1.520601844193056</v>
+        <v>1.520601844193057</v>
       </c>
       <c r="E6">
         <v>-10.40025407585737</v>
       </c>
       <c r="F6">
-        <v>0.8312050572165446</v>
+        <v>0.8312050572165448</v>
       </c>
       <c r="G6">
-        <v>-8.380174487851768</v>
+        <v>-8.380174487851772</v>
       </c>
       <c r="H6">
-        <v>0.03729585551908479</v>
+        <v>0.03729585551908485</v>
       </c>
       <c r="I6">
-        <v>-0.7175660235358906</v>
+        <v>-0.7175660235358907</v>
       </c>
       <c r="J6">
-        <v>-0.06508710207152611</v>
+        <v>-0.06508710207152604</v>
       </c>
       <c r="K6">
         <v>0.8982796489936381</v>
       </c>
       <c r="L6">
-        <v>-0.3688488178457793</v>
+        <v>-0.3688488178457792</v>
       </c>
       <c r="M6">
-        <v>2.79181280931899</v>
+        <v>2.791812809318989</v>
       </c>
       <c r="N6">
-        <v>0.2857434155902019</v>
+        <v>0.2857434155902008</v>
       </c>
       <c r="O6">
-        <v>-1.556032338575846</v>
+        <v>-1.556032338575843</v>
       </c>
       <c r="P6">
-        <v>-0.07246337697313605</v>
+        <v>-0.07246337697313572</v>
       </c>
       <c r="Q6">
-        <v>0.2088441934989191</v>
+        <v>0.2088441934989194</v>
       </c>
       <c r="R6">
         <v>9999.686604517508</v>
@@ -1066,46 +1066,46 @@
         <v>2880.334169928937</v>
       </c>
       <c r="D7">
-        <v>8.030666472195492</v>
+        <v>8.030666472195493</v>
       </c>
       <c r="E7">
         <v>-102.9681621161403</v>
       </c>
       <c r="F7">
-        <v>-0.4769441691336769</v>
+        <v>-0.4769441691336742</v>
       </c>
       <c r="G7">
         <v>-40.71443721306763</v>
       </c>
       <c r="H7">
-        <v>0.3413972027342612</v>
+        <v>0.3413972027342639</v>
       </c>
       <c r="I7">
-        <v>-19.00848016858873</v>
+        <v>-19.00848016858874</v>
       </c>
       <c r="J7">
-        <v>0.04071829421918825</v>
+        <v>0.04071829421919065</v>
       </c>
       <c r="K7">
         <v>-6.083976774271058</v>
       </c>
       <c r="L7">
-        <v>-0.06643334236929041</v>
+        <v>-0.0664333423692916</v>
       </c>
       <c r="M7">
-        <v>-1.45411138237078</v>
+        <v>-1.454111382370782</v>
       </c>
       <c r="N7">
-        <v>-0.195431006606372</v>
+        <v>-0.1954310066064042</v>
       </c>
       <c r="O7">
-        <v>-0.3914503066764011</v>
+        <v>-0.3914503066763195</v>
       </c>
       <c r="P7">
-        <v>0.0007658153403677705</v>
+        <v>0.0007658153403914023</v>
       </c>
       <c r="Q7">
-        <v>-0.09094516599223262</v>
+        <v>-0.09094516599222514</v>
       </c>
       <c r="R7">
         <v>3924.583743737668</v>
@@ -1164,46 +1164,46 @@
         <v>421.7675412068219</v>
       </c>
       <c r="D8">
-        <v>3.933099578022457</v>
+        <v>3.933099578022456</v>
       </c>
       <c r="E8">
         <v>-98.22389278735834</v>
       </c>
       <c r="F8">
-        <v>-0.4499586647880943</v>
+        <v>-0.4499586647880926</v>
       </c>
       <c r="G8">
-        <v>-8.964821934890297</v>
+        <v>-8.964821934890303</v>
       </c>
       <c r="H8">
-        <v>0.005872665162180496</v>
+        <v>0.005872665162181086</v>
       </c>
       <c r="I8">
-        <v>0.2780706887266789</v>
+        <v>0.2780706887266786</v>
       </c>
       <c r="J8">
-        <v>-0.108679837962031</v>
+        <v>-0.1086798379620302</v>
       </c>
       <c r="K8">
-        <v>0.359144459087455</v>
+        <v>0.3591444590874575</v>
       </c>
       <c r="L8">
-        <v>0.00744575824645229</v>
+        <v>0.007445758246456468</v>
       </c>
       <c r="M8">
-        <v>0.3494774226299343</v>
+        <v>0.3494774226299476</v>
       </c>
       <c r="N8">
-        <v>0.1645153716248129</v>
+        <v>0.1645153716247875</v>
       </c>
       <c r="O8">
-        <v>-0.3461642553629748</v>
+        <v>-0.3461642553630373</v>
       </c>
       <c r="P8">
-        <v>-0.0002162807604464084</v>
+        <v>-0.0002162807604438962</v>
       </c>
       <c r="Q8">
-        <v>-0.1234300518457799</v>
+        <v>-0.1234300518457798</v>
       </c>
       <c r="R8">
         <v>1.629919257347524</v>

</xml_diff>